<commit_message>
avancement upload de fichier
</commit_message>
<xml_diff>
--- a/documents/Projet.xlsx
+++ b/documents/Projet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Soumission Candidature" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Conception du formulaire d'inscription</t>
   </si>
@@ -137,16 +137,13 @@
     <t>Détail de la candidature</t>
   </si>
   <si>
-    <t>Cas d'erreur lorsque la candidature est non conforme + commentaire</t>
-  </si>
-  <si>
-    <t>cases à cocher d'erreur par information</t>
-  </si>
-  <si>
-    <t>Récapitulation des erreurs en bas de page</t>
-  </si>
-  <si>
     <t>Récupération filière par web service</t>
+  </si>
+  <si>
+    <t>Commentaire Erreur</t>
+  </si>
+  <si>
+    <t>ce champ doit resté fixe en scrollant</t>
   </si>
 </sst>
 </file>
@@ -636,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
@@ -767,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -842,33 +839,21 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>